<commit_message>
Used standard names for all countries
</commit_message>
<xml_diff>
--- a/docs/African_Languages.xlsx
+++ b/docs/African_Languages.xlsx
@@ -18483,7 +18483,7 @@
       </c>
       <c r="D821" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18505,7 +18505,7 @@
       </c>
       <c r="D822" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18527,7 +18527,7 @@
       </c>
       <c r="D823" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18549,7 +18549,7 @@
       </c>
       <c r="D824" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18571,7 +18571,7 @@
       </c>
       <c r="D825" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18593,7 +18593,7 @@
       </c>
       <c r="D826" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18615,7 +18615,7 @@
       </c>
       <c r="D827" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18637,7 +18637,7 @@
       </c>
       <c r="D828" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18659,7 +18659,7 @@
       </c>
       <c r="D829" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18681,7 +18681,7 @@
       </c>
       <c r="D830" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18703,7 +18703,7 @@
       </c>
       <c r="D831" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18725,7 +18725,7 @@
       </c>
       <c r="D832" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18747,7 +18747,7 @@
       </c>
       <c r="D833" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18769,7 +18769,7 @@
       </c>
       <c r="D834" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18791,7 +18791,7 @@
       </c>
       <c r="D835" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18813,7 +18813,7 @@
       </c>
       <c r="D836" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18835,7 +18835,7 @@
       </c>
       <c r="D837" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18857,7 +18857,7 @@
       </c>
       <c r="D838" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18879,7 +18879,7 @@
       </c>
       <c r="D839" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18901,7 +18901,7 @@
       </c>
       <c r="D840" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18923,7 +18923,7 @@
       </c>
       <c r="D841" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18945,7 +18945,7 @@
       </c>
       <c r="D842" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18967,7 +18967,7 @@
       </c>
       <c r="D843" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -18989,7 +18989,7 @@
       </c>
       <c r="D844" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19011,7 +19011,7 @@
       </c>
       <c r="D845" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19033,7 +19033,7 @@
       </c>
       <c r="D846" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19055,7 +19055,7 @@
       </c>
       <c r="D847" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19077,7 +19077,7 @@
       </c>
       <c r="D848" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19099,7 +19099,7 @@
       </c>
       <c r="D849" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19121,7 +19121,7 @@
       </c>
       <c r="D850" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19143,7 +19143,7 @@
       </c>
       <c r="D851" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19165,7 +19165,7 @@
       </c>
       <c r="D852" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19187,7 +19187,7 @@
       </c>
       <c r="D853" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19209,7 +19209,7 @@
       </c>
       <c r="D854" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19231,7 +19231,7 @@
       </c>
       <c r="D855" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19253,7 +19253,7 @@
       </c>
       <c r="D856" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19275,7 +19275,7 @@
       </c>
       <c r="D857" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19297,7 +19297,7 @@
       </c>
       <c r="D858" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19319,7 +19319,7 @@
       </c>
       <c r="D859" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19341,7 +19341,7 @@
       </c>
       <c r="D860" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19363,7 +19363,7 @@
       </c>
       <c r="D861" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19385,7 +19385,7 @@
       </c>
       <c r="D862" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19407,7 +19407,7 @@
       </c>
       <c r="D863" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19429,7 +19429,7 @@
       </c>
       <c r="D864" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19451,7 +19451,7 @@
       </c>
       <c r="D865" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19473,7 +19473,7 @@
       </c>
       <c r="D866" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19495,7 +19495,7 @@
       </c>
       <c r="D867" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19517,7 +19517,7 @@
       </c>
       <c r="D868" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19539,7 +19539,7 @@
       </c>
       <c r="D869" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19561,7 +19561,7 @@
       </c>
       <c r="D870" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19583,7 +19583,7 @@
       </c>
       <c r="D871" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19605,7 +19605,7 @@
       </c>
       <c r="D872" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19627,7 +19627,7 @@
       </c>
       <c r="D873" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19649,7 +19649,7 @@
       </c>
       <c r="D874" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19671,7 +19671,7 @@
       </c>
       <c r="D875" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19693,7 +19693,7 @@
       </c>
       <c r="D876" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19715,7 +19715,7 @@
       </c>
       <c r="D877" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19737,7 +19737,7 @@
       </c>
       <c r="D878" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19759,7 +19759,7 @@
       </c>
       <c r="D879" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19781,7 +19781,7 @@
       </c>
       <c r="D880" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19803,7 +19803,7 @@
       </c>
       <c r="D881" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19825,7 +19825,7 @@
       </c>
       <c r="D882" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19847,7 +19847,7 @@
       </c>
       <c r="D883" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19869,7 +19869,7 @@
       </c>
       <c r="D884" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19891,7 +19891,7 @@
       </c>
       <c r="D885" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19913,7 +19913,7 @@
       </c>
       <c r="D886" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19935,7 +19935,7 @@
       </c>
       <c r="D887" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19957,7 +19957,7 @@
       </c>
       <c r="D888" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -19979,7 +19979,7 @@
       </c>
       <c r="D889" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20001,7 +20001,7 @@
       </c>
       <c r="D890" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20023,7 +20023,7 @@
       </c>
       <c r="D891" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20045,7 +20045,7 @@
       </c>
       <c r="D892" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20067,7 +20067,7 @@
       </c>
       <c r="D893" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20089,7 +20089,7 @@
       </c>
       <c r="D894" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20111,7 +20111,7 @@
       </c>
       <c r="D895" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20133,7 +20133,7 @@
       </c>
       <c r="D896" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20155,7 +20155,7 @@
       </c>
       <c r="D897" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20177,7 +20177,7 @@
       </c>
       <c r="D898" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20199,7 +20199,7 @@
       </c>
       <c r="D899" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20221,7 +20221,7 @@
       </c>
       <c r="D900" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20243,7 +20243,7 @@
       </c>
       <c r="D901" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20265,7 +20265,7 @@
       </c>
       <c r="D902" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20287,7 +20287,7 @@
       </c>
       <c r="D903" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20309,7 +20309,7 @@
       </c>
       <c r="D904" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20331,7 +20331,7 @@
       </c>
       <c r="D905" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20353,7 +20353,7 @@
       </c>
       <c r="D906" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20375,7 +20375,7 @@
       </c>
       <c r="D907" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20397,7 +20397,7 @@
       </c>
       <c r="D908" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20419,7 +20419,7 @@
       </c>
       <c r="D909" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20441,7 +20441,7 @@
       </c>
       <c r="D910" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20463,7 +20463,7 @@
       </c>
       <c r="D911" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20485,7 +20485,7 @@
       </c>
       <c r="D912" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20507,7 +20507,7 @@
       </c>
       <c r="D913" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20529,7 +20529,7 @@
       </c>
       <c r="D914" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20551,7 +20551,7 @@
       </c>
       <c r="D915" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20573,7 +20573,7 @@
       </c>
       <c r="D916" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20595,7 +20595,7 @@
       </c>
       <c r="D917" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20617,7 +20617,7 @@
       </c>
       <c r="D918" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20639,7 +20639,7 @@
       </c>
       <c r="D919" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20661,7 +20661,7 @@
       </c>
       <c r="D920" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20683,7 +20683,7 @@
       </c>
       <c r="D921" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20705,7 +20705,7 @@
       </c>
       <c r="D922" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20727,7 +20727,7 @@
       </c>
       <c r="D923" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20749,7 +20749,7 @@
       </c>
       <c r="D924" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20771,7 +20771,7 @@
       </c>
       <c r="D925" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20793,7 +20793,7 @@
       </c>
       <c r="D926" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20815,7 +20815,7 @@
       </c>
       <c r="D927" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20837,7 +20837,7 @@
       </c>
       <c r="D928" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20859,7 +20859,7 @@
       </c>
       <c r="D929" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20881,7 +20881,7 @@
       </c>
       <c r="D930" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20903,7 +20903,7 @@
       </c>
       <c r="D931" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20925,7 +20925,7 @@
       </c>
       <c r="D932" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20947,7 +20947,7 @@
       </c>
       <c r="D933" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20969,7 +20969,7 @@
       </c>
       <c r="D934" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -20991,7 +20991,7 @@
       </c>
       <c r="D935" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21013,7 +21013,7 @@
       </c>
       <c r="D936" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21035,7 +21035,7 @@
       </c>
       <c r="D937" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21057,7 +21057,7 @@
       </c>
       <c r="D938" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21079,7 +21079,7 @@
       </c>
       <c r="D939" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21101,7 +21101,7 @@
       </c>
       <c r="D940" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21123,7 +21123,7 @@
       </c>
       <c r="D941" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21145,7 +21145,7 @@
       </c>
       <c r="D942" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21167,7 +21167,7 @@
       </c>
       <c r="D943" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21189,7 +21189,7 @@
       </c>
       <c r="D944" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21211,7 +21211,7 @@
       </c>
       <c r="D945" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21233,7 +21233,7 @@
       </c>
       <c r="D946" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21255,7 +21255,7 @@
       </c>
       <c r="D947" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21277,7 +21277,7 @@
       </c>
       <c r="D948" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21299,7 +21299,7 @@
       </c>
       <c r="D949" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21321,7 +21321,7 @@
       </c>
       <c r="D950" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21343,7 +21343,7 @@
       </c>
       <c r="D951" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21365,7 +21365,7 @@
       </c>
       <c r="D952" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21387,7 +21387,7 @@
       </c>
       <c r="D953" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21409,7 +21409,7 @@
       </c>
       <c r="D954" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21431,7 +21431,7 @@
       </c>
       <c r="D955" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21453,7 +21453,7 @@
       </c>
       <c r="D956" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21475,7 +21475,7 @@
       </c>
       <c r="D957" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21497,7 +21497,7 @@
       </c>
       <c r="D958" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21519,7 +21519,7 @@
       </c>
       <c r="D959" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21541,7 +21541,7 @@
       </c>
       <c r="D960" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21563,7 +21563,7 @@
       </c>
       <c r="D961" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21585,7 +21585,7 @@
       </c>
       <c r="D962" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21607,7 +21607,7 @@
       </c>
       <c r="D963" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21629,7 +21629,7 @@
       </c>
       <c r="D964" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21651,7 +21651,7 @@
       </c>
       <c r="D965" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21673,7 +21673,7 @@
       </c>
       <c r="D966" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21695,7 +21695,7 @@
       </c>
       <c r="D967" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21717,7 +21717,7 @@
       </c>
       <c r="D968" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21739,7 +21739,7 @@
       </c>
       <c r="D969" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21761,7 +21761,7 @@
       </c>
       <c r="D970" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21783,7 +21783,7 @@
       </c>
       <c r="D971" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21805,7 +21805,7 @@
       </c>
       <c r="D972" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21827,7 +21827,7 @@
       </c>
       <c r="D973" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21849,7 +21849,7 @@
       </c>
       <c r="D974" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21871,7 +21871,7 @@
       </c>
       <c r="D975" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21893,7 +21893,7 @@
       </c>
       <c r="D976" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21915,7 +21915,7 @@
       </c>
       <c r="D977" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21937,7 +21937,7 @@
       </c>
       <c r="D978" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21959,7 +21959,7 @@
       </c>
       <c r="D979" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -21981,7 +21981,7 @@
       </c>
       <c r="D980" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22003,7 +22003,7 @@
       </c>
       <c r="D981" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22025,7 +22025,7 @@
       </c>
       <c r="D982" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22047,7 +22047,7 @@
       </c>
       <c r="D983" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22069,7 +22069,7 @@
       </c>
       <c r="D984" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22091,7 +22091,7 @@
       </c>
       <c r="D985" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22113,7 +22113,7 @@
       </c>
       <c r="D986" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22135,7 +22135,7 @@
       </c>
       <c r="D987" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22157,7 +22157,7 @@
       </c>
       <c r="D988" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22179,7 +22179,7 @@
       </c>
       <c r="D989" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22201,7 +22201,7 @@
       </c>
       <c r="D990" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22223,7 +22223,7 @@
       </c>
       <c r="D991" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22245,7 +22245,7 @@
       </c>
       <c r="D992" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22267,7 +22267,7 @@
       </c>
       <c r="D993" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22289,7 +22289,7 @@
       </c>
       <c r="D994" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22311,7 +22311,7 @@
       </c>
       <c r="D995" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22333,7 +22333,7 @@
       </c>
       <c r="D996" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22355,7 +22355,7 @@
       </c>
       <c r="D997" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22377,7 +22377,7 @@
       </c>
       <c r="D998" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22399,7 +22399,7 @@
       </c>
       <c r="D999" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22421,7 +22421,7 @@
       </c>
       <c r="D1000" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22443,7 +22443,7 @@
       </c>
       <c r="D1001" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22465,7 +22465,7 @@
       </c>
       <c r="D1002" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22487,7 +22487,7 @@
       </c>
       <c r="D1003" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22509,7 +22509,7 @@
       </c>
       <c r="D1004" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22531,7 +22531,7 @@
       </c>
       <c r="D1005" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22553,7 +22553,7 @@
       </c>
       <c r="D1006" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22575,7 +22575,7 @@
       </c>
       <c r="D1007" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22597,7 +22597,7 @@
       </c>
       <c r="D1008" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22619,7 +22619,7 @@
       </c>
       <c r="D1009" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22641,7 +22641,7 @@
       </c>
       <c r="D1010" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22663,7 +22663,7 @@
       </c>
       <c r="D1011" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22685,7 +22685,7 @@
       </c>
       <c r="D1012" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22707,7 +22707,7 @@
       </c>
       <c r="D1013" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22729,7 +22729,7 @@
       </c>
       <c r="D1014" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22751,7 +22751,7 @@
       </c>
       <c r="D1015" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22773,7 +22773,7 @@
       </c>
       <c r="D1016" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22795,7 +22795,7 @@
       </c>
       <c r="D1017" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22817,7 +22817,7 @@
       </c>
       <c r="D1018" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22839,7 +22839,7 @@
       </c>
       <c r="D1019" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22861,7 +22861,7 @@
       </c>
       <c r="D1020" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22883,7 +22883,7 @@
       </c>
       <c r="D1021" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22905,7 +22905,7 @@
       </c>
       <c r="D1022" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22927,7 +22927,7 @@
       </c>
       <c r="D1023" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22949,7 +22949,7 @@
       </c>
       <c r="D1024" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22971,7 +22971,7 @@
       </c>
       <c r="D1025" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -22993,7 +22993,7 @@
       </c>
       <c r="D1026" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -23015,7 +23015,7 @@
       </c>
       <c r="D1027" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -23037,7 +23037,7 @@
       </c>
       <c r="D1028" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>
@@ -23051,7 +23051,7 @@
       </c>
       <c r="D1029" t="inlineStr">
         <is>
-          <t>Congo, The Democratic Republic of the</t>
+          <t>Democratic Republic of Congo</t>
         </is>
       </c>
     </row>

</xml_diff>